<commit_message>
changed y-axis, added more details
</commit_message>
<xml_diff>
--- a/Plots/predictability_sheet_chart.xlsx
+++ b/Plots/predictability_sheet_chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soroush/Box Sync/05_Proposals (Review-Submitted)/01_Submitted Proposals/CPS_2018_codes/Plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228AB8B0-5F4B-AE41-B0A6-0BBCA5794C34}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA7FA89-0D19-D346-85EB-51EA5849BFAB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" activeTab="5" xr2:uid="{AF2D054C-3F52-4E6B-9D28-BE5AE247C88F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14340" activeTab="6" xr2:uid="{AF2D054C-3F52-4E6B-9D28-BE5AE247C88F}"/>
   </bookViews>
   <sheets>
     <sheet name="wenjing" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="2 chal (hd=5)" sheetId="3" r:id="rId4"/>
     <sheet name="5 chal" sheetId="4" r:id="rId5"/>
     <sheet name="all" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>dec</t>
   </si>
@@ -95,25 +96,73 @@
     <t>rel HD (0,4)</t>
   </si>
   <si>
-    <t>Closeness</t>
-  </si>
-  <si>
     <t># challenges</t>
   </si>
   <si>
     <t>predictability</t>
   </si>
   <si>
-    <t>center</t>
+    <t>[0,5)</t>
   </si>
   <si>
-    <t>1 chal</t>
+    <t>[75,85)</t>
   </si>
   <si>
-    <t>2 chal</t>
+    <t>[65,75)</t>
   </si>
   <si>
-    <t>5 chal</t>
+    <t>[55,65)</t>
+  </si>
+  <si>
+    <t>[45,55)</t>
+  </si>
+  <si>
+    <t>[35,45)</t>
+  </si>
+  <si>
+    <t>[25,35)</t>
+  </si>
+  <si>
+    <t>[15,25)</t>
+  </si>
+  <si>
+    <t>[5,15)</t>
+  </si>
+  <si>
+    <t>[85,95)</t>
+  </si>
+  <si>
+    <t>[95,100]</t>
+  </si>
+  <si>
+    <t>[50,60)</t>
+  </si>
+  <si>
+    <t>[60,70)</t>
+  </si>
+  <si>
+    <t>[70,80)</t>
+  </si>
+  <si>
+    <t>[80,90)</t>
+  </si>
+  <si>
+    <t>[90,100)</t>
+  </si>
+  <si>
+    <t>[0.5,0.6)</t>
+  </si>
+  <si>
+    <t>[0.6,0.7)</t>
+  </si>
+  <si>
+    <t>[0.7,0.8)</t>
+  </si>
+  <si>
+    <t>[0.9,1.0)</t>
+  </si>
+  <si>
+    <t>[0.8,0.9)</t>
   </si>
 </sst>
 </file>
@@ -37204,15 +37253,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3894CED-6364-854A-BD5A-AFA90D39A3E2}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E6"/>
+      <selection activeCell="B2" sqref="B2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -37222,106 +37271,118 @@
       <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
-        <f>A2/4</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B6" si="0">A3/4</f>
-        <v>0.25</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>16</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D6" si="1">(2/PI())*ATAN(SQRT(8-B3)/SQRT(B3))</f>
-        <v>0.88686591774267887</v>
-      </c>
-      <c r="E3">
-        <f>E2+SUM(C2:C3)/2</f>
-        <v>10</v>
+        <f>(2/PI())*ATAN(SQRT(8-A3)/SQRT(A3))</f>
+        <v>0.76994654383738415</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C10" si="0">(2/PI())*ATAN(SQRT(8-A4)/SQRT(A4))</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>56</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0.58043062325516626</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>70</v>
+      </c>
+      <c r="C6">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="C4">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
         <v>56</v>
       </c>
-      <c r="D4">
-        <f t="shared" si="1"/>
-        <v>0.8391387534896676</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E6" si="2">E3+SUM(C3:C4)/2</f>
-        <v>46</v>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0.4195693767448338</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>28</v>
+      </c>
+      <c r="C8">
         <f t="shared" si="0"/>
-        <v>0.75</v>
-      </c>
-      <c r="C5">
-        <v>112</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="1"/>
-        <v>0.80189395724367352</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="2"/>
-        <v>130</v>
+        <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>70</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="1"/>
-        <v>0.76994654383738415</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="2"/>
-        <v>221</v>
+        <v>0.23005345616261588</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <f>SUM(B2:B10)</f>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -37331,15 +37392,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D5C7CC-AFC7-EC44-8E5B-DA190A648561}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E6"/>
+      <selection activeCell="B2" sqref="B2:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -37349,105 +37410,117 @@
       <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
-        <f>A2/4</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B6" si="0">A3/4</f>
-        <v>0.25</v>
+        <v>14</v>
       </c>
       <c r="C3">
-        <v>28</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D6" si="1">(2/PI())*ATAN(SQRT(8-B3)/SQRT(B3))</f>
-        <v>0.88686591774267887</v>
-      </c>
-      <c r="E3">
-        <f>E2+SUM(C2:C3)/2</f>
-        <v>18</v>
+        <f>(2/PI())*ATAN(SQRT(8-A3)/SQRT(A3))</f>
+        <v>0.76994654383738415</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
+        <v>42</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C10" si="0">(2/PI())*ATAN(SQRT(8-A4)/SQRT(A4))</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>70</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0.58043062325516626</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="C4">
-        <v>84</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="1"/>
-        <v>0.8391387534896676</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E6" si="2">E3+SUM(C3:C4)/2</f>
-        <v>74</v>
-      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>70</v>
+      </c>
+      <c r="C7">
         <f t="shared" si="0"/>
-        <v>0.75</v>
-      </c>
-      <c r="C5">
-        <v>140</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="1"/>
-        <v>0.80189395724367352</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="2"/>
-        <v>186</v>
+        <v>0.4195693767448338</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>42</v>
+      </c>
+      <c r="C8">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="1"/>
-        <v>0.76994654383738415</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="2"/>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0.23005345616261588</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <f>SUM(B2:B10)</f>
         <v>256</v>
       </c>
     </row>
@@ -37458,15 +37531,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A41BE5-AE4B-3647-85AD-FF234C478E25}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -37476,105 +37549,113 @@
       <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
-        <f>A2/4</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B6" si="0">A3/4</f>
-        <v>0.25</v>
-      </c>
-      <c r="C3">
-        <v>32</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D6" si="1">(2/PI())*ATAN(SQRT(8-B3)/SQRT(B3))</f>
-        <v>0.88686591774267887</v>
-      </c>
-      <c r="E3">
-        <f>E2+SUM(C2:C3)/2</f>
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
+        <v>50</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C10" si="0">(2/PI())*ATAN(SQRT(8-A4)/SQRT(A4))</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>60</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0.58043062325516626</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="C4">
-        <v>100</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="1"/>
-        <v>0.8391387534896676</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E6" si="2">E3+SUM(C3:C4)/2</f>
-        <v>86</v>
-      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>60</v>
+      </c>
+      <c r="C7">
         <f t="shared" si="0"/>
-        <v>0.75</v>
-      </c>
-      <c r="C5">
-        <v>120</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="1"/>
-        <v>0.80189395724367352</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="2"/>
-        <v>196</v>
+        <v>0.4195693767448338</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>50</v>
+      </c>
+      <c r="C8">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="1"/>
-        <v>0.76994654383738415</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="2"/>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0.23005345616261588</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <f>SUM(B2:B10)</f>
         <v>256</v>
       </c>
     </row>
@@ -37585,15 +37666,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75F0E079-9FDE-4240-9496-408D18E5206A}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E6"/>
+      <selection activeCell="B2" sqref="B2:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -37603,105 +37684,117 @@
       <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
-        <f>A2/4</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B6" si="0">A3/4</f>
-        <v>0.25</v>
+        <v>38</v>
       </c>
       <c r="C3">
-        <v>76</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D6" si="1">(2/PI())*ATAN(SQRT(8-B3)/SQRT(B3))</f>
-        <v>0.88686591774267887</v>
-      </c>
-      <c r="E3">
-        <f>E2+SUM(C2:C3)/2</f>
-        <v>48</v>
+        <f>(2/PI())*ATAN(SQRT(8-A3)/SQRT(A3))</f>
+        <v>0.76994654383738415</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
+        <v>64</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C10" si="0">(2/PI())*ATAN(SQRT(8-A4)/SQRT(A4))</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0.58043062325516626</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="C4">
-        <v>128</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="1"/>
-        <v>0.8391387534896676</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E6" si="2">E3+SUM(C3:C4)/2</f>
-        <v>150</v>
-      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>21</v>
+      </c>
+      <c r="C7">
         <f t="shared" si="0"/>
-        <v>0.75</v>
-      </c>
-      <c r="C5">
-        <v>42</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="1"/>
-        <v>0.80189395724367352</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="2"/>
-        <v>235</v>
+        <v>0.4195693767448338</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>64</v>
+      </c>
+      <c r="C8">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="1"/>
-        <v>0.76994654383738415</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="2"/>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>38</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0.23005345616261588</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <f>SUM(B2:B10)</f>
         <v>256</v>
       </c>
     </row>
@@ -37712,221 +37805,634 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48CE1A59-D03C-1944-8A10-492D19E14A0D}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" t="s">
-        <v>27</v>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="J1">
+        <v>5</v>
+      </c>
+      <c r="K1">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
+      <c r="A2" t="s">
+        <v>31</v>
       </c>
       <c r="B2">
-        <f>A2/4</f>
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>4</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="K2">
-        <v>5</v>
+        <v>0.76994654383738415</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
+      <c r="A3" t="s">
+        <v>30</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B6" si="0">A3/4</f>
-        <v>0.25</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>0.88686591774267887</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <v>16</v>
       </c>
       <c r="E3">
-        <v>10</v>
-      </c>
-      <c r="F3">
-        <v>28</v>
-      </c>
-      <c r="G3">
-        <v>18</v>
-      </c>
-      <c r="H3">
-        <v>32</v>
-      </c>
-      <c r="I3">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="J3">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="K3">
-        <v>48</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2</v>
+      <c r="A4" t="s">
+        <v>29</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>28</v>
       </c>
       <c r="C4">
-        <v>0.8391387534896676</v>
+        <v>42</v>
       </c>
       <c r="D4">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E4">
-        <v>46</v>
-      </c>
-      <c r="F4">
-        <v>84</v>
-      </c>
-      <c r="G4">
-        <v>74</v>
-      </c>
-      <c r="H4">
-        <v>100</v>
-      </c>
-      <c r="I4">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="J4">
-        <v>128</v>
+        <v>21</v>
       </c>
       <c r="K4">
-        <v>150</v>
+        <v>0.58043062325516626</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>3</v>
+      <c r="A5" t="s">
+        <v>28</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>56</v>
       </c>
       <c r="C5">
-        <v>0.80189395724367352</v>
+        <v>70</v>
       </c>
       <c r="D5">
-        <v>112</v>
+        <v>60</v>
       </c>
       <c r="E5">
-        <v>130</v>
-      </c>
-      <c r="F5">
-        <v>140</v>
-      </c>
-      <c r="G5">
-        <v>186</v>
-      </c>
-      <c r="H5">
-        <v>120</v>
-      </c>
-      <c r="I5">
-        <v>196</v>
+        <v>21</v>
       </c>
       <c r="J5">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>235</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6">
+        <v>70</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>21</v>
+      </c>
+      <c r="K6">
+        <v>0.4195693767448338</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>56</v>
+      </c>
+      <c r="C7">
+        <v>70</v>
+      </c>
+      <c r="D7">
+        <v>60</v>
+      </c>
+      <c r="E7">
+        <v>21</v>
+      </c>
+      <c r="J7">
+        <v>64</v>
+      </c>
+      <c r="K7">
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>28</v>
+      </c>
+      <c r="C8">
+        <v>42</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
+      <c r="E8">
+        <v>64</v>
+      </c>
+      <c r="J8">
+        <v>38</v>
+      </c>
+      <c r="K8">
+        <v>0.23005345616261588</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>38</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17">
+        <f>SUM(B5:B7)</f>
+        <v>182</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:E17" si="0">SUM(C5:C7)</f>
+        <v>140</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18">
+        <f>B8*2</f>
+        <v>56</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:E18" si="1">C8*2</f>
+        <v>84</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19">
+        <f>B9*2</f>
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ref="C19:E19" si="2">C9*2</f>
+        <v>28</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21">
+        <f>B11*2</f>
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21:E21" si="3">C11*2</f>
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="D21">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D715FB-0CD6-114C-8BF2-08A3D1C9D1BF}">
+  <dimension ref="A1:O11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1">
+        <f>L6+L5</f>
+        <v>672</v>
+      </c>
+      <c r="C1">
+        <f t="shared" ref="C1:E1" si="0">M6+M5</f>
+        <v>504</v>
+      </c>
+      <c r="D1">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>0.76994654383738415</v>
-      </c>
-      <c r="D6">
-        <v>70</v>
-      </c>
-      <c r="E6">
-        <v>221</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>256</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
+        <v>400</v>
+      </c>
+      <c r="E1">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="I1">
+        <v>0</v>
+      </c>
+      <c r="J1">
+        <v>1</v>
+      </c>
+      <c r="L1">
+        <v>2</v>
+      </c>
+      <c r="M1">
+        <v>4</v>
+      </c>
+      <c r="N1">
+        <v>4</v>
+      </c>
+      <c r="O1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2">
+        <f>L4</f>
+        <v>240</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:E2" si="1">M4</f>
+        <v>336</v>
+      </c>
+      <c r="D2">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="E2">
+        <f t="shared" si="1"/>
+        <v>436</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <f>(2/PI())*ATAN(SQRT(11-I2)/SQRT(I2))</f>
+        <v>0.80501777095786342</v>
+      </c>
+      <c r="L2">
+        <v>20</v>
+      </c>
+      <c r="M2">
+        <v>36</v>
+      </c>
+      <c r="N2">
+        <v>40</v>
+      </c>
+      <c r="O2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3">
+        <f>L3</f>
+        <v>90</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:E3" si="2">M3</f>
+        <v>144</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="2"/>
+        <v>390</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J11" si="3">(2/PI())*ATAN(SQRT(11-I3)/SQRT(I3))</f>
+        <v>0.71956220199245657</v>
+      </c>
+      <c r="L3">
+        <v>90</v>
+      </c>
+      <c r="M3">
+        <v>144</v>
+      </c>
+      <c r="N3">
+        <v>180</v>
+      </c>
+      <c r="O3">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4">
+        <f>L2</f>
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:E4" si="4">M2</f>
+        <v>36</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="3"/>
+        <v>0.65019828771895727</v>
+      </c>
+      <c r="L4">
+        <v>240</v>
+      </c>
+      <c r="M4">
+        <v>336</v>
+      </c>
+      <c r="N4">
+        <v>400</v>
+      </c>
+      <c r="O4">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5">
+        <f>L1</f>
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:E5" si="5">M1</f>
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="3"/>
+        <v>0.58792566739929086</v>
+      </c>
+      <c r="L5">
+        <v>420</v>
+      </c>
+      <c r="M5">
+        <v>364</v>
+      </c>
+      <c r="N5">
+        <v>400</v>
+      </c>
+      <c r="O5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I6">
-        <v>256</v>
+        <v>5</v>
       </c>
       <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>256</v>
+        <f t="shared" si="3"/>
+        <v>0.52897726983585625</v>
+      </c>
+      <c r="L6">
+        <v>252</v>
+      </c>
+      <c r="M6">
+        <v>140</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>0.47102273016414387</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <v>7</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>0.41207433260070919</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>0.34980171228104284</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I10">
+        <v>9</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>0.28043779800754354</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>0.19498222904213666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>